<commit_message>
adding work class n6
</commit_message>
<xml_diff>
--- a/Clases grabadas FrontEnd.xlsx
+++ b/Clases grabadas FrontEnd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebas\OneDrive\Escritorio\Programacion\Clases UTN repaso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD17D27B-8C4B-4308-A238-73226AEE7CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F8AB1D-FD3C-4AE8-9C5D-20140E31BC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -294,7 +294,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,6 +328,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,7 +465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -532,6 +538,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -816,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z982"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,6 +834,7 @@
     <col min="1" max="1" width="15.5546875" customWidth="1"/>
     <col min="2" max="2" width="10.109375" customWidth="1"/>
     <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
     <col min="5" max="5" width="105" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1160,7 +1170,9 @@
       <c r="C10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="25">
+        <v>6.6666666666666666E-2</v>
+      </c>
       <c r="E10" s="11" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
adding ColorHunt in CSS proyect
</commit_message>
<xml_diff>
--- a/Clases grabadas FrontEnd.xlsx
+++ b/Clases grabadas FrontEnd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebas\OneDrive\Escritorio\Programacion\Clases UTN repaso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64AF6D5-14B9-461E-8B3F-7E4C3B956D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EF57BB-728B-44FA-9674-E4B0F153A177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -294,7 +294,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,12 +328,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,7 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -538,9 +532,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -825,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z982"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1284,9 +1275,7 @@
       <c r="C13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="25">
-        <v>4.3749999999999997E-2</v>
-      </c>
+      <c r="D13" s="19"/>
       <c r="E13" s="11" t="s">
         <v>27</v>
       </c>
@@ -1326,7 +1315,7 @@
       <c r="C14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="11" t="s">
         <v>29</v>
       </c>

</xml_diff>